<commit_message>
Completed ISXEQ2 and EQ2 TLOs. Adding Tracing to all members and methods.
</commit_message>
<xml_diff>
--- a/ISXEQ2 Documentation.xlsx
+++ b/ISXEQ2 Documentation.xlsx
@@ -12,10 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Item" sheetId="1" r:id="rId1"/>
+    <sheet name="ISXEQ2" sheetId="3" r:id="rId1"/>
+    <sheet name="EQ2" sheetId="2" r:id="rId2"/>
+    <sheet name="Item" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Item!$E$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Item!$F$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="207">
   <si>
     <t>IsQuestItemUsable</t>
   </si>
@@ -356,9 +358,6 @@
     <t>float</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -435,6 +434,222 @@
   </si>
   <si>
     <t>Initialize</t>
+  </si>
+  <si>
+    <t>DEPRECATED</t>
+  </si>
+  <si>
+    <t>ItemModifier</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Returns MaxRange</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>OnBattleGround</t>
+  </si>
+  <si>
+    <t>ServerName</t>
+  </si>
+  <si>
+    <t>CustomActorArraySize</t>
+  </si>
+  <si>
+    <t>Zoning</t>
+  </si>
+  <si>
+    <t>HOWindowActive</t>
+  </si>
+  <si>
+    <t>HOName</t>
+  </si>
+  <si>
+    <t>HODescription</t>
+  </si>
+  <si>
+    <t>HOWheelID</t>
+  </si>
+  <si>
+    <t>HOWindowState</t>
+  </si>
+  <si>
+    <t>HOTimeLimit</t>
+  </si>
+  <si>
+    <t>HOTimeElapsed</t>
+  </si>
+  <si>
+    <t>HOTimeRemaining</t>
+  </si>
+  <si>
+    <t>HOLastManipulator</t>
+  </si>
+  <si>
+    <t>HOCurrentWheelSlot</t>
+  </si>
+  <si>
+    <t>HOWheelState</t>
+  </si>
+  <si>
+    <t>HOIconID1</t>
+  </si>
+  <si>
+    <t>HOIconID2</t>
+  </si>
+  <si>
+    <t>HOIconID3</t>
+  </si>
+  <si>
+    <t>HOIconID4</t>
+  </si>
+  <si>
+    <t>HOIconID5</t>
+  </si>
+  <si>
+    <t>HOIconID6</t>
+  </si>
+  <si>
+    <t>NumRadars</t>
+  </si>
+  <si>
+    <t>MasterVolume</t>
+  </si>
+  <si>
+    <t>RK</t>
+  </si>
+  <si>
+    <t>InRoomID</t>
+  </si>
+  <si>
+    <t>PendingQuestName</t>
+  </si>
+  <si>
+    <t>PendingQuestDescription</t>
+  </si>
+  <si>
+    <t>InboxMailCount</t>
+  </si>
+  <si>
+    <t>RewardPending</t>
+  </si>
+  <si>
+    <t>CheckCollision</t>
+  </si>
+  <si>
+    <t>HeadingTo</t>
+  </si>
+  <si>
+    <t>PersistentZoneID</t>
+  </si>
+  <si>
+    <t>CreateCustomActorArray</t>
+  </si>
+  <si>
+    <t>SetMasterVolume</t>
+  </si>
+  <si>
+    <t>AcceptPendingQuest</t>
+  </si>
+  <si>
+    <t>DeclinePendingQuest</t>
+  </si>
+  <si>
+    <t>SetAmbientLight</t>
+  </si>
+  <si>
+    <t>AcceptReward</t>
+  </si>
+  <si>
+    <t>ConfirmZoneTeleporterDestination</t>
+  </si>
+  <si>
+    <t>ShowAllOnScreenAnnouncements</t>
+  </si>
+  <si>
+    <t>GetPersistentZones</t>
+  </si>
+  <si>
+    <t>GetActors</t>
+  </si>
+  <si>
+    <t>Only available while in the game proper.</t>
+  </si>
+  <si>
+    <t>actor</t>
+  </si>
+  <si>
+    <t>NotUsed</t>
+  </si>
+  <si>
+    <t>Not Used</t>
+  </si>
+  <si>
+    <t>uint</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>EQ2LocsCount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AfflictionEventsOn             </t>
+  </si>
+  <si>
+    <t>IsValidEQ2PressKey</t>
+  </si>
+  <si>
+    <t>InitializingActorEffects</t>
+  </si>
+  <si>
+    <t>SetActorEventsRange</t>
+  </si>
+  <si>
+    <t>ResetInternalVendingSystem</t>
+  </si>
+  <si>
+    <t>EnableAfflictionEvents</t>
+  </si>
+  <si>
+    <t>EB</t>
+  </si>
+  <si>
+    <t>AddLoc</t>
+  </si>
+  <si>
+    <t>DisableAfflictionEvents</t>
+  </si>
+  <si>
+    <t>EnduringBreath</t>
+  </si>
+  <si>
+    <t>Popup</t>
+  </si>
+  <si>
+    <t>SetAfflictionEventsTimeInterval</t>
+  </si>
+  <si>
+    <t>NoFog</t>
+  </si>
+  <si>
+    <t>EnableActorEvents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ClearAbilitiesCache                   </t>
+  </si>
+  <si>
+    <t>SetActorEventsTimeInterval</t>
+  </si>
+  <si>
+    <t>DisableActorEvents</t>
   </si>
 </sst>
 </file>
@@ -764,10 +979,1015 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="F8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="F9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="F10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="F11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="F12" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="F13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="F14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="F15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="F2:F15">
+    <sortCondition ref="F2:F15"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G106"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="6" max="6" width="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="F2:F11">
+    <sortCondition ref="F2:F11"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G106"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,11 +1995,12 @@
     <col min="1" max="1" width="22" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="4" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>105</v>
       </c>
@@ -787,16 +2008,19 @@
         <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>93</v>
       </c>
@@ -804,13 +2028,13 @@
         <v>106</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>101</v>
       </c>
@@ -818,13 +2042,13 @@
         <v>106</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>79</v>
       </c>
@@ -832,13 +2056,13 @@
         <v>106</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>77</v>
       </c>
@@ -846,13 +2070,13 @@
         <v>106</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>76</v>
       </c>
@@ -860,13 +2084,13 @@
         <v>106</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>96</v>
       </c>
@@ -874,13 +2098,13 @@
         <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>61</v>
       </c>
@@ -888,13 +2112,13 @@
         <v>107</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
@@ -902,13 +2126,13 @@
         <v>107</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -916,13 +2140,13 @@
         <v>106</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
@@ -930,13 +2154,13 @@
         <v>106</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>71</v>
       </c>
@@ -944,13 +2168,13 @@
         <v>108</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E12" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -958,27 +2182,27 @@
         <v>107</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>46</v>
       </c>
@@ -986,13 +2210,13 @@
         <v>107</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -1000,13 +2224,13 @@
         <v>107</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>98</v>
       </c>
@@ -1014,27 +2238,27 @@
         <v>106</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E17" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
@@ -1042,41 +2266,41 @@
         <v>108</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>64</v>
       </c>
@@ -1084,24 +2308,24 @@
         <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="F22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>56</v>
       </c>
@@ -1109,32 +2333,32 @@
         <v>108</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>87</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>97</v>
       </c>
@@ -1142,21 +2366,21 @@
         <v>107</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>100</v>
       </c>
@@ -1164,21 +2388,21 @@
         <v>106</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>99</v>
       </c>
@@ -1186,10 +2410,10 @@
         <v>106</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>103</v>
       </c>
@@ -1197,7 +2421,7 @@
         <v>106</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1208,7 +2432,7 @@
         <v>107</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1219,7 +2443,7 @@
         <v>106</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1230,7 +2454,7 @@
         <v>106</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1241,7 +2465,7 @@
         <v>107</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1252,7 +2476,7 @@
         <v>107</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1263,7 +2487,7 @@
         <v>106</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1274,7 +2498,7 @@
         <v>106</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1285,7 +2509,7 @@
         <v>106</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1296,7 +2520,7 @@
         <v>106</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1307,7 +2531,7 @@
         <v>106</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1318,7 +2542,7 @@
         <v>106</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1329,7 +2553,7 @@
         <v>106</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1340,7 +2564,7 @@
         <v>106</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1351,7 +2575,7 @@
         <v>106</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1362,7 +2586,7 @@
         <v>106</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1373,7 +2597,7 @@
         <v>106</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1384,7 +2608,7 @@
         <v>106</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1395,7 +2619,7 @@
         <v>106</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1406,7 +2630,7 @@
         <v>106</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1417,7 +2641,7 @@
         <v>106</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1427,6 +2651,9 @@
       <c r="B53" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="C53" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
@@ -1435,6 +2662,9 @@
       <c r="B54" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="C54" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -1443,266 +2673,566 @@
       <c r="B55" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="C55" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="B56" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="B57" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>55</v>
       </c>
+      <c r="B58" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B59" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="B60" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>102</v>
       </c>
+      <c r="B61" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="B62" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="B63" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D90" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>38</v>
       </c>
+      <c r="B106" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:F1">
-    <sortState ref="E2:F22">
-      <sortCondition ref="E1"/>
+  <autoFilter ref="F1:G1">
+    <sortState ref="F2:G22">
+      <sortCondition ref="F1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed update of ChoiceWindow, Consignment, EQ2Mail, EQ2UIElements, EQ2UIPage, Merchandise, Radar, VendingContainer, Vendor, and Zone. Created a class sharing all methods and members in common between Merchandise and Consignment (VendorItem) to resolve the VendingContainer member "Item(int or string)".
</commit_message>
<xml_diff>
--- a/ISXEQ2 Documentation.xlsx
+++ b/ISXEQ2 Documentation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raymond\Source\Repos\ISXEQ2Wrapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanere\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" tabRatio="876" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" tabRatio="876" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Ability" sheetId="4" r:id="rId1"/>
@@ -22,15 +22,18 @@
     <sheet name="EQ2" sheetId="2" r:id="rId8"/>
     <sheet name="EQ2Location" sheetId="6" r:id="rId9"/>
     <sheet name="EQ2Mail" sheetId="7" r:id="rId10"/>
-    <sheet name="ISXEQ2" sheetId="3" r:id="rId11"/>
-    <sheet name="Item" sheetId="1" r:id="rId12"/>
-    <sheet name="Maintained" sheetId="12" r:id="rId13"/>
-    <sheet name="Merchandise" sheetId="16" r:id="rId14"/>
-    <sheet name="Radar" sheetId="8" r:id="rId15"/>
-    <sheet name="Recipe" sheetId="14" r:id="rId16"/>
+    <sheet name="EQ2UIElement" sheetId="19" r:id="rId11"/>
+    <sheet name="ISXEQ2" sheetId="3" r:id="rId12"/>
+    <sheet name="Item" sheetId="1" r:id="rId13"/>
+    <sheet name="Maintained" sheetId="12" r:id="rId14"/>
+    <sheet name="Merchandise" sheetId="16" r:id="rId15"/>
+    <sheet name="Radar" sheetId="8" r:id="rId16"/>
+    <sheet name="Recipe" sheetId="14" r:id="rId17"/>
+    <sheet name="VendingContainer" sheetId="17" r:id="rId18"/>
+    <sheet name="Vendor" sheetId="18" r:id="rId19"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Item!$F$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Item!$F$1:$G$1</definedName>
     <definedName name="Ability" localSheetId="0">Ability!$A$1:$D$12</definedName>
     <definedName name="AbilityEffect" localSheetId="1">AbilityEffect!$A$2:$D$3</definedName>
     <definedName name="Achievement" localSheetId="2">Achievement!$A$2:$D$5</definedName>
@@ -38,10 +41,13 @@
     <definedName name="Consignment" localSheetId="5">Consignment!$A$2:$F$2</definedName>
     <definedName name="Effect" localSheetId="6">Effect!$A$2:$D$5</definedName>
     <definedName name="EQ2Mail" localSheetId="9">EQ2Mail!$A$2:$F$4</definedName>
-    <definedName name="Maintained" localSheetId="12">Maintained!$A$2:$D$5</definedName>
-    <definedName name="Merchandise" localSheetId="13">Merchandise!$A$2:$E$6</definedName>
-    <definedName name="Radar" localSheetId="14">Radar!$A$2:$E$13</definedName>
-    <definedName name="Recipe" localSheetId="15">Recipe!$A$2:$C$9</definedName>
+    <definedName name="EQ2UIElement" localSheetId="10">EQ2UIElement!$A$2:$F$6</definedName>
+    <definedName name="Maintained" localSheetId="13">Maintained!$A$2:$D$5</definedName>
+    <definedName name="Merchandise" localSheetId="14">Merchandise!$A$2:$E$6</definedName>
+    <definedName name="Radar" localSheetId="15">Radar!$A$2:$E$13</definedName>
+    <definedName name="Recipe" localSheetId="16">Recipe!$A$2:$C$9</definedName>
+    <definedName name="VendingContainer" localSheetId="17">VendingContainer!$A$2:$E$5</definedName>
+    <definedName name="Vendor" localSheetId="18">Vendor!$A$2:$E$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -129,7 +135,19 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="Maintained" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="8" name="EQ2UIElement" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\EQ2UIElement.txt" delimited="0">
+      <textFields count="6">
+        <textField/>
+        <textField position="17"/>
+        <textField position="34"/>
+        <textField position="51"/>
+        <textField position="68"/>
+        <textField position="85"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="Maintained" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Maintained.txt" delimited="0">
       <textFields count="4">
         <textField/>
@@ -139,7 +157,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="Merchandise" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="10" name="Merchandise" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\raymond\Source\Repos\ISXEQ2Wrapper\Merchandise.txt" delimited="0">
       <textFields count="5">
         <textField/>
@@ -150,7 +168,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="Radar" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="11" name="Radar" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Radar.txt" delimited="0">
       <textFields count="5">
         <textField/>
@@ -161,7 +179,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="Recipe" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="12" name="Recipe" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Recipe.txt" delimited="0">
       <textFields count="3">
         <textField/>
@@ -170,11 +188,33 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="13" name="VendingContainer" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\VendingContainer.txt" delimited="0">
+      <textFields count="5">
+        <textField/>
+        <textField position="15"/>
+        <textField position="30"/>
+        <textField position="45"/>
+        <textField position="60"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="14" name="Vendor" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Vendor.txt" delimited="0">
+      <textFields count="5">
+        <textField/>
+        <textField position="20"/>
+        <textField position="40"/>
+        <textField position="60"/>
+        <textField position="74"/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="548">
   <si>
     <t>IsQuestItemUsable</t>
   </si>
@@ -1706,13 +1746,118 @@
     <t>StatusCost</t>
   </si>
   <si>
-    <t>Sell</t>
-  </si>
-  <si>
-    <t>ListForSale</t>
-  </si>
-  <si>
-    <t>UnListForSale</t>
+    <t>TotalCapacity</t>
+  </si>
+  <si>
+    <t>TotalCoin</t>
+  </si>
+  <si>
+    <t>NumItems</t>
+  </si>
+  <si>
+    <t>UsedCapacity</t>
+  </si>
+  <si>
+    <t>CurrentCoin</t>
+  </si>
+  <si>
+    <t>Consignment</t>
+  </si>
+  <si>
+    <t>TakeCoin</t>
+  </si>
+  <si>
+    <t>ChangeTo</t>
+  </si>
+  <si>
+    <t>int64</t>
+  </si>
+  <si>
+    <t>NumItemsForSale</t>
+  </si>
+  <si>
+    <t>CurrentSearchPage</t>
+  </si>
+  <si>
+    <t>Merchant</t>
+  </si>
+  <si>
+    <t>IsBroker</t>
+  </si>
+  <si>
+    <t>Commission</t>
+  </si>
+  <si>
+    <t>TotalSearchPages</t>
+  </si>
+  <si>
+    <t>Broker</t>
+  </si>
+  <si>
+    <t>IsMerchant</t>
+  </si>
+  <si>
+    <t>GotoSearchPage</t>
+  </si>
+  <si>
+    <t>Merchandise or Consignment</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>ChildType</t>
+  </si>
+  <si>
+    <t>ShortLabel</t>
+  </si>
+  <si>
+    <t>RowHighlighted</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>IsChecked</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>IsSet</t>
+  </si>
+  <si>
+    <t>Percent</t>
+  </si>
+  <si>
+    <t>NumChildren</t>
+  </si>
+  <si>
+    <t>GetDynamicData</t>
+  </si>
+  <si>
+    <t>IsEnabled</t>
+  </si>
+  <si>
+    <t>ClickButton</t>
+  </si>
+  <si>
+    <t>RightClick</t>
+  </si>
+  <si>
+    <t>LeftClick</t>
+  </si>
+  <si>
+    <t>DoubleLeftClick</t>
+  </si>
+  <si>
+    <t>AddToTextBox</t>
+  </si>
+  <si>
+    <t>HighlightRow</t>
+  </si>
+  <si>
+    <t>EQ2UIElement</t>
   </si>
 </sst>
 </file>
@@ -1748,7 +1893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1777,6 +1922,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1799,11 +1947,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Radar" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Merchandise" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Recipe" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Radar" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Recipe" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="VendingContainer" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Vendor" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1831,11 +1991,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Maintained" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="EQ2UIElement" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Merchandise" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Maintained" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2837,7 +2997,7 @@
   <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,6 +3037,9 @@
       <c r="B2" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>395</v>
       </c>
@@ -2888,6 +3051,9 @@
       <c r="B3" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>391</v>
       </c>
@@ -2899,6 +3065,9 @@
       <c r="B4" s="4" t="s">
         <v>137</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>396</v>
       </c>
@@ -2910,6 +3079,9 @@
       <c r="B5" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>401</v>
       </c>
@@ -2921,6 +3093,9 @@
       <c r="B6" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>400</v>
       </c>
@@ -2932,6 +3107,9 @@
       <c r="B7" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>389</v>
       </c>
@@ -2943,6 +3121,9 @@
       <c r="B8" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F8" s="3" t="s">
         <v>394</v>
       </c>
@@ -2954,6 +3135,9 @@
       <c r="B9" s="4" t="s">
         <v>109</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F9" t="s">
         <v>393</v>
       </c>
@@ -2965,6 +3149,9 @@
       <c r="B10" s="4" t="s">
         <v>107</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>381</v>
       </c>
@@ -2975,6 +3162,9 @@
       </c>
       <c r="B11" s="4" t="s">
         <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>123</v>
@@ -3218,6 +3408,400 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G145"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>539</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F4" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>540</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="F2:F145">
+    <sortCondition ref="F2:F145"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -3671,7 +4255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -4923,7 +5507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -5367,12 +5951,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
+  <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5384,9 +5968,10 @@
     <col min="5" max="5" width="9.140625" style="8"/>
     <col min="6" max="6" width="13.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>105</v>
       </c>
@@ -5406,7 +5991,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>508</v>
       </c>
@@ -5416,8 +6001,12 @@
       <c r="F2" s="8" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="2"/>
+      <c r="J2" s="3" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
@@ -5430,8 +6019,14 @@
       <c r="F3" s="8" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -5441,22 +6036,21 @@
       <c r="C4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>507</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -5466,22 +6060,24 @@
       <c r="C6" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>497</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>506</v>
       </c>
@@ -5489,15 +6085,18 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>509</v>
       </c>
@@ -5505,7 +6104,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -5515,20 +6114,24 @@
       <c r="C11" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -5809,7 +6412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -6377,12 +6980,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6874,6 +7477,863 @@
     </row>
   </sheetData>
   <sortState ref="A2:C106">
+    <sortCondition ref="A2:A106"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G106"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>515</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>513</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="F2:F4">
+    <sortCondition ref="F2:F4"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G106"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="F2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B106">
     <sortCondition ref="A2:A106"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8761,7 +10221,7 @@
   <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Continued work on Actor.
</commit_message>
<xml_diff>
--- a/ISXEQ2 Documentation.xlsx
+++ b/ISXEQ2 Documentation.xlsx
@@ -58,7 +58,6 @@
     <definedName name="Vendor" localSheetId="22">Vendor!$A$2:$E$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -268,7 +267,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="667">
   <si>
     <t>IsQuestItemUsable</t>
   </si>
@@ -2361,12 +2360,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11033,13 +11028,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" style="8" customWidth="1"/>
@@ -11069,254 +11064,305 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>1</v>
+        <v>589</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>654</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>568</v>
+        <v>170</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>657</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>382</v>
+        <v>626</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>261</v>
+        <v>656</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>658</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>254</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F5" s="3" t="s">
-        <v>626</v>
+        <v>379</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>616</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>295</v>
+        <v>622</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>633</v>
+        <v>108</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>303</v>
+        <v>584</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>634</v>
+        <v>109</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>629</v>
       </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>55</v>
+        <v>635</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>107</v>
+        <v>636</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>637</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>287</v>
+        <v>578</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>640</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>2</v>
+        <v>583</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>255</v>
+        <v>575</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="D12" s="8" t="s">
+        <v>660</v>
+      </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>112</v>
+        <v>645</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>108</v>
+        <v>220</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>646</v>
       </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>258</v>
+        <v>287</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>171</v>
+        <v>574</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>324</v>
+        <v>576</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>661</v>
+        <v>109</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>617</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>605</v>
+        <v>261</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>612</v>
+        <v>591</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>618</v>
+        <v>324</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>562</v>
+        <v>171</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>569</v>
+        <v>295</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>604</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>576</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>628</v>
+      <c r="D24" s="8" t="s">
+        <v>664</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>584</v>
+        <v>2</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>635</v>
+        <v>586</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>636</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>637</v>
+        <v>106</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>317</v>
+        <v>611</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>106</v>
@@ -11324,10 +11370,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>325</v>
+        <v>599</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>106</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -11337,10 +11389,13 @@
       <c r="B29" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="C29" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>106</v>
@@ -11348,80 +11403,89 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>345</v>
+        <v>600</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>474</v>
+        <v>587</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>476</v>
+        <v>106</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>563</v>
+        <v>588</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>570</v>
+        <v>345</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>630</v>
+        <v>106</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>577</v>
+        <v>598</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>585</v>
+        <v>603</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>596</v>
+        <v>566</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>632</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>600</v>
+        <v>569</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>106</v>
@@ -11429,416 +11493,415 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>607</v>
+        <v>562</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="C40" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>106</v>
       </c>
+      <c r="D41" s="8" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>619</v>
+        <v>594</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>564</v>
+        <v>618</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>571</v>
+        <v>602</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>578</v>
+        <v>642</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>640</v>
+        <v>106</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D46" s="11" t="s">
-        <v>641</v>
+      <c r="D46" s="8" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>592</v>
+        <v>609</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D47" s="11"/>
+      <c r="D47" s="8" t="s">
+        <v>650</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D48" s="11"/>
+      <c r="C48" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>601</v>
+        <v>325</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D49" s="11" t="s">
-        <v>641</v>
+      <c r="C49" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="11"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>614</v>
+        <v>563</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D51" s="11"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>620</v>
+        <v>526</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="11"/>
+      <c r="C52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>648</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>565</v>
+        <v>607</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D53" s="11" t="s">
-        <v>641</v>
+      <c r="C53" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>572</v>
+        <v>613</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D54" s="11"/>
+      <c r="C54" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D55" s="11"/>
+      <c r="D55" s="12" t="s">
+        <v>654</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>587</v>
+        <v>565</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D56" s="8" t="s">
         <v>641</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>593</v>
+        <v>297</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="11"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>597</v>
+        <v>612</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D58" s="11"/>
+      <c r="C58" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>602</v>
+        <v>579</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D59" s="11"/>
-    </row>
-    <row r="60" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>642</v>
+        <v>580</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D60" s="8" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>318</v>
+        <v>593</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>644</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>86</v>
+        <v>597</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>645</v>
+        <v>619</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>646</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D64" s="8" t="s">
-        <v>649</v>
-      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>647</v>
+        <v>109</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>588</v>
+        <v>55</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>526</v>
+        <v>621</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D67" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>598</v>
+        <v>1</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>106</v>
+        <v>109</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>603</v>
+        <v>86</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>615</v>
+        <v>623</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>651</v>
+        <v>665</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>652</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>566</v>
+        <v>620</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>574</v>
+        <v>608</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>581</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>589</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>654</v>
+      <c r="D76" s="8" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>594</v>
+        <v>254</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>249</v>
+        <v>585</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>170</v>
+        <v>596</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>656</v>
+        <v>564</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D80" s="5" t="s">
-        <v>658</v>
+        <v>108</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>610</v>
+        <v>474</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>108</v>
+        <v>476</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>108</v>
@@ -11846,111 +11909,105 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>622</v>
+        <v>590</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>567</v>
+        <v>595</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>660</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>582</v>
+        <v>249</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>107</v>
+        <v>476</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>590</v>
+        <v>39</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>595</v>
+        <v>567</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="300" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>599</v>
+        <v>577</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>663</v>
+        <v>109</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>604</v>
+        <v>570</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D90" s="8" t="s">
-        <v>664</v>
+        <v>630</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>611</v>
+        <v>255</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
-        <v>617</v>
-      </c>
-      <c r="D92" s="6" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>665</v>
+        <v>258</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="D56:D59"/>
-  </mergeCells>
+  <sortState ref="F2:F93">
+    <sortCondition ref="F2:F93"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Approximately 45% complete with Character.
</commit_message>
<xml_diff>
--- a/ISXEQ2 Documentation.xlsx
+++ b/ISXEQ2 Documentation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" tabRatio="876" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" tabRatio="876" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ability" sheetId="4" r:id="rId1"/>
@@ -24,20 +24,21 @@
     <sheet name="EQ2Location" sheetId="6" r:id="rId10"/>
     <sheet name="EQ2Mail" sheetId="7" r:id="rId11"/>
     <sheet name="EQ2UIElement" sheetId="19" r:id="rId12"/>
-    <sheet name="ISXEQ2" sheetId="3" r:id="rId13"/>
-    <sheet name="Item" sheetId="1" r:id="rId14"/>
-    <sheet name="LootWindow" sheetId="20" r:id="rId15"/>
-    <sheet name="Maintained" sheetId="12" r:id="rId16"/>
-    <sheet name="Merchandise" sheetId="16" r:id="rId17"/>
-    <sheet name="Radar" sheetId="8" r:id="rId18"/>
-    <sheet name="Recipe" sheetId="14" r:id="rId19"/>
-    <sheet name="ReplyDialog" sheetId="21" r:id="rId20"/>
-    <sheet name="RewardWindow" sheetId="22" r:id="rId21"/>
-    <sheet name="VendingContainer" sheetId="17" r:id="rId22"/>
-    <sheet name="Vendor" sheetId="18" r:id="rId23"/>
+    <sheet name="GroupMember" sheetId="24" r:id="rId13"/>
+    <sheet name="ISXEQ2" sheetId="3" r:id="rId14"/>
+    <sheet name="Item" sheetId="1" r:id="rId15"/>
+    <sheet name="LootWindow" sheetId="20" r:id="rId16"/>
+    <sheet name="Maintained" sheetId="12" r:id="rId17"/>
+    <sheet name="Merchandise" sheetId="16" r:id="rId18"/>
+    <sheet name="Radar" sheetId="8" r:id="rId19"/>
+    <sheet name="Recipe" sheetId="14" r:id="rId20"/>
+    <sheet name="ReplyDialog" sheetId="21" r:id="rId21"/>
+    <sheet name="RewardWindow" sheetId="22" r:id="rId22"/>
+    <sheet name="VendingContainer" sheetId="17" r:id="rId23"/>
+    <sheet name="Vendor" sheetId="18" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Item!$F$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Item!$F$1:$G$1</definedName>
     <definedName name="Ability" localSheetId="0">Ability!$A$1:$D$12</definedName>
     <definedName name="AbilityEffect" localSheetId="1">AbilityEffect!$A$2:$D$3</definedName>
     <definedName name="Achievement" localSheetId="2">Achievement!$A$2:$D$5</definedName>
@@ -47,15 +48,16 @@
     <definedName name="Effect" localSheetId="7">Effect!$A$2:$D$5</definedName>
     <definedName name="EQ2Mail" localSheetId="10">EQ2Mail!$A$2:$F$4</definedName>
     <definedName name="EQ2UIElement" localSheetId="11">EQ2UIElement!$A$2:$F$6</definedName>
-    <definedName name="LootWindow" localSheetId="14">LootWindow!$A$2:$G$4</definedName>
-    <definedName name="Maintained" localSheetId="15">Maintained!$A$2:$D$5</definedName>
-    <definedName name="Merchandise" localSheetId="16">Merchandise!$A$2:$E$6</definedName>
-    <definedName name="Radar" localSheetId="17">Radar!$A$2:$E$13</definedName>
-    <definedName name="Recipe" localSheetId="18">Recipe!$A$2:$C$9</definedName>
-    <definedName name="ReplyDialog" localSheetId="19">ReplyDialog!$A$2:$B$4</definedName>
-    <definedName name="RewardWindow" localSheetId="20">RewardWindow!$A$2:$C$4</definedName>
-    <definedName name="VendingContainer" localSheetId="21">VendingContainer!$A$2:$E$5</definedName>
-    <definedName name="Vendor" localSheetId="22">Vendor!$A$2:$E$5</definedName>
+    <definedName name="GroupMember" localSheetId="12">GroupMember!$A$2:$G$4</definedName>
+    <definedName name="LootWindow" localSheetId="15">LootWindow!$A$2:$G$4</definedName>
+    <definedName name="Maintained" localSheetId="16">Maintained!$A$2:$D$5</definedName>
+    <definedName name="Merchandise" localSheetId="17">Merchandise!$A$2:$E$6</definedName>
+    <definedName name="Radar" localSheetId="18">Radar!$A$2:$E$13</definedName>
+    <definedName name="Recipe" localSheetId="19">Recipe!$A$2:$C$9</definedName>
+    <definedName name="ReplyDialog" localSheetId="20">ReplyDialog!$A$2:$B$4</definedName>
+    <definedName name="RewardWindow" localSheetId="21">RewardWindow!$A$2:$C$4</definedName>
+    <definedName name="VendingContainer" localSheetId="22">VendingContainer!$A$2:$E$5</definedName>
+    <definedName name="Vendor" localSheetId="23">Vendor!$A$2:$E$5</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -170,7 +172,20 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="LootWindow" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="10" name="GroupMember" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\raymond\Source\Repos\ISXEQ2Wrapper\GroupMember.txt" delimited="0">
+      <textFields count="7">
+        <textField/>
+        <textField position="23"/>
+        <textField position="46"/>
+        <textField position="69"/>
+        <textField position="92"/>
+        <textField position="115"/>
+        <textField position="138"/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="11" name="LootWindow" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\raymond\Source\Repos\ISXEQ2Wrapper\LootWindow.txt" delimited="0">
       <textFields count="7">
         <textField/>
@@ -183,7 +198,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="Maintained" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="12" name="Maintained" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Maintained.txt" delimited="0">
       <textFields count="4">
         <textField/>
@@ -193,7 +208,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="Merchandise" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="13" name="Merchandise" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\raymond\Source\Repos\ISXEQ2Wrapper\Merchandise.txt" delimited="0">
       <textFields count="5">
         <textField/>
@@ -204,7 +219,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="13" name="Radar" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="14" name="Radar" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Radar.txt" delimited="0">
       <textFields count="5">
         <textField/>
@@ -215,7 +230,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="14" name="Recipe" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="15" name="Recipe" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Recipe.txt" delimited="0">
       <textFields count="3">
         <textField/>
@@ -224,7 +239,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="15" name="ReplyDialog" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="16" name="ReplyDialog" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\raymond\Source\Repos\ISXEQ2Wrapper\ReplyDialog.txt" space="1" consecutive="1">
       <textFields count="2">
         <textField/>
@@ -232,7 +247,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="16" name="RewardWindow" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="17" name="RewardWindow" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\raymond\Source\Repos\ISXEQ2Wrapper\RewardWindow.txt" delimited="0">
       <textFields count="3">
         <textField/>
@@ -241,7 +256,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="17" name="VendingContainer" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="18" name="VendingContainer" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\VendingContainer.txt" delimited="0">
       <textFields count="5">
         <textField/>
@@ -252,7 +267,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="18" name="Vendor" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="19" name="Vendor" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\lanere\Source\Repos\ISXEQ2Wrapper\Vendor.txt" delimited="0">
       <textFields count="5">
         <textField/>
@@ -267,7 +282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1609" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="678">
   <si>
     <t>IsQuestItemUsable</t>
   </si>
@@ -2285,6 +2300,39 @@
   </si>
   <si>
     <t>You're currently flying in the air using a flying mount (the mount is visible)</t>
+  </si>
+  <si>
+    <t>HitPoints</t>
+  </si>
+  <si>
+    <t>MaxHitPoints</t>
+  </si>
+  <si>
+    <t>PetID</t>
+  </si>
+  <si>
+    <t>RaidRole</t>
+  </si>
+  <si>
+    <t>ZoneName</t>
+  </si>
+  <si>
+    <t>int, GroupMember</t>
+  </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>IEnumerable&lt;Ability&gt;</t>
+  </si>
+  <si>
+    <t>IEnumerable&lt;Item&gt;</t>
+  </si>
+  <si>
+    <t>GroupMember</t>
+  </si>
+  <si>
+    <t>VendingContainer</t>
   </si>
 </sst>
 </file>
@@ -2384,39 +2432,43 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LootWindow" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="GroupMember" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Maintained" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="LootWindow" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Merchandise" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Maintained" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Radar" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Merchandise" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Recipe" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Radar" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ReplyDialog" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Recipe" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RewardWindow" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ReplyDialog" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="VendingContainer" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RewardWindow" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Vendor" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="VendingContainer" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Vendor" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4196,7 +4248,7 @@
   <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4586,6 +4638,436 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G145"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="3"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="3"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="3"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="3"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="3"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="3"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="3"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="3"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="3"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="3"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="3"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="3"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="3"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="3"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="3"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="3"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="3"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="3"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="3"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:C145">
+    <sortCondition ref="A2:A145"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -5039,7 +5521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -6291,7 +6773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -6698,7 +7180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -7142,7 +7624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J106"/>
   <sheetViews>
@@ -7603,7 +8085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -8166,509 +8648,6 @@
   </sheetData>
   <sortState ref="F2:G106">
     <sortCondition ref="F2:F106"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G106"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="34" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>488</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>493</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>483</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="3"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="3"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="3"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="3"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="3"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="3"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="3"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="3"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="3"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="3"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="3"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="3"/>
-    </row>
-  </sheetData>
-  <sortState ref="A2:C106">
-    <sortCondition ref="A2:A106"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9072,6 +9051,509 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="34" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3"/>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="3"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="3"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="3"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="3"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="3"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="3"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="3"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="3"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="3"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="3"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="3"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="3"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="3"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="3"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="3"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:C106">
+    <sortCondition ref="A2:A106"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G106"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
     <col min="1" max="1" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -9436,7 +9918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -9808,7 +10290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -10250,7 +10732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G106"/>
   <sheetViews>
@@ -11028,8 +11510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11860,6 +12342,9 @@
       <c r="B77" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="C77" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
@@ -11876,6 +12361,9 @@
       <c r="B79" s="1" t="s">
         <v>109</v>
       </c>
+      <c r="C79" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="D79" s="11" t="s">
         <v>632</v>
       </c>
@@ -11887,6 +12375,9 @@
       <c r="B80" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="C80" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="D80" s="8" t="s">
         <v>638</v>
       </c>
@@ -11906,6 +12397,9 @@
       <c r="B82" s="1" t="s">
         <v>108</v>
       </c>
+      <c r="C82" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
@@ -11948,6 +12442,9 @@
       </c>
       <c r="B87" s="1" t="s">
         <v>109</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -12017,14 +12514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
@@ -12055,6 +12552,9 @@
       <c r="A2" s="3" t="s">
         <v>273</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>273</v>
+      </c>
       <c r="F2" s="3" t="s">
         <v>376</v>
       </c>
@@ -12063,6 +12563,9 @@
       <c r="A3" s="2" t="s">
         <v>260</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>260</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>378</v>
       </c>
@@ -12071,6 +12574,9 @@
       <c r="A4" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>371</v>
       </c>
@@ -12079,6 +12585,9 @@
       <c r="A5" s="2" t="s">
         <v>250</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>373</v>
       </c>
@@ -12087,6 +12596,9 @@
       <c r="A6" s="3" t="s">
         <v>364</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F6" s="3" t="s">
         <v>368</v>
       </c>
@@ -12095,6 +12607,9 @@
       <c r="A7" s="3" t="s">
         <v>362</v>
       </c>
+      <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F7" s="3" t="s">
         <v>369</v>
       </c>
@@ -12103,6 +12618,9 @@
       <c r="A8" s="2" t="s">
         <v>236</v>
       </c>
+      <c r="B8" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="F8" s="3" t="s">
         <v>372</v>
       </c>
@@ -12111,6 +12629,12 @@
       <c r="A9" s="3" t="s">
         <v>264</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F9" s="3" t="s">
         <v>379</v>
       </c>
@@ -12119,6 +12643,9 @@
       <c r="A10" s="2" t="s">
         <v>338</v>
       </c>
+      <c r="B10" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="F10" s="3" t="s">
         <v>370</v>
       </c>
@@ -12127,6 +12654,9 @@
       <c r="A11" s="3" t="s">
         <v>252</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>106</v>
+      </c>
       <c r="F11" s="3" t="s">
         <v>375</v>
       </c>
@@ -12135,6 +12665,9 @@
       <c r="A12" s="2" t="s">
         <v>310</v>
       </c>
+      <c r="B12" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="F12" s="3" t="s">
         <v>377</v>
       </c>
@@ -12143,6 +12676,12 @@
       <c r="A13" s="3" t="s">
         <v>344</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="F13" s="3" t="s">
         <v>374</v>
       </c>
@@ -12151,675 +12690,1089 @@
       <c r="A14" s="3" t="s">
         <v>351</v>
       </c>
+      <c r="B14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>340</v>
       </c>
+      <c r="B15" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>258</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>